<commit_message>
code polishing, removed mention of old scripts
</commit_message>
<xml_diff>
--- a/tests/3_MAG_confrontation_and_final_results/MAG_FINAL_RESULTS.xlsx
+++ b/tests/3_MAG_confrontation_and_final_results/MAG_FINAL_RESULTS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="MAG hits" sheetId="1" state="visible" r:id="rId2"/>
@@ -73,34 +73,34 @@
     <t xml:space="preserve">KO</t>
   </si>
   <si>
-    <t xml:space="preserve">seq0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xseq0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seq1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xseq1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seq2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xseq2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">len_prodigal_xseq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">len_xseq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">len_xseq1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">len_xseq2</t>
+    <t xml:space="preserve">seq_no_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translated_seq_no_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seq_70%_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translated_seq_70%_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seq_30%_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translated_seq_30%_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">len_prodigal_translated_seq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">len_translated_seq_no_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">len_translated_seq_70%_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">len_translated_seq_30%_deletion</t>
   </si>
   <si>
     <t xml:space="preserve">xseq2 &gt; xseq1</t>
@@ -118,22 +118,22 @@
     <t xml:space="preserve">prodigal_contig</t>
   </si>
   <si>
-    <t xml:space="preserve">0_contig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1_contig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2_contig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0_contig AS pr_contig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1_contig AS pr_contig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2_contig AS pr_contig</t>
+    <t xml:space="preserve">contig_no_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contig_70%_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contig_30%_deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contig_no_del = pr_contig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contig_70%_del = pr_contig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contig_30%_del = pr_contig</t>
   </si>
   <si>
     <t xml:space="preserve">prodigal_strand</t>
@@ -806,7 +806,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1307,37 +1306,35 @@
   </sheetPr>
   <dimension ref="A1:BA39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AS39" activeCellId="0" sqref="AS39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BA2" activeCellId="0" sqref="BA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.14795918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.05102040816327"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="20" min="18" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="24" min="21" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="27" min="25" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="31" min="28" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="34" min="32" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="37" min="36" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="41" min="39" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="44" min="42" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="46" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="20" min="18" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="24" min="21" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="27" min="25" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="31" min="28" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="34" min="32" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="37" min="36" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="41" min="39" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="44" min="42" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="46" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7209,40 +7206,40 @@
         <v>0.0434782608695652</v>
       </c>
       <c r="AS39" s="57" t="n">
-        <f aca="false">SUM(AS3:AS38)/23</f>
-        <v>0.869565217391304</v>
+        <f aca="false">SUM(AS3:AS38)/36</f>
+        <v>0.555555555555556</v>
       </c>
       <c r="AT39" s="57" t="n">
-        <f aca="false">SUM(AT3:AT38)/23</f>
-        <v>0.217391304347826</v>
+        <f aca="false">SUM(AT3:AT38)/36</f>
+        <v>0.138888888888889</v>
       </c>
       <c r="AU39" s="57" t="n">
-        <f aca="false">SUM(AU3:AU38)/23</f>
-        <v>0.652173913043478</v>
+        <f aca="false">SUM(AU3:AU38)/36</f>
+        <v>0.416666666666667</v>
       </c>
       <c r="AV39" s="57" t="n">
-        <f aca="false">SUM(AV3:AV38)/23</f>
+        <f aca="false">SUM(AV3:AV38)/36</f>
         <v>0</v>
       </c>
       <c r="AW39" s="57" t="n">
-        <f aca="false">SUM(AW3:AW38)/23</f>
-        <v>0.0869565217391304</v>
+        <f aca="false">SUM(AW3:AW38)/36</f>
+        <v>0.0555555555555556</v>
       </c>
       <c r="AX39" s="57" t="n">
-        <f aca="false">SUM(AX3:AX38)/23</f>
-        <v>0.0434782608695652</v>
+        <f aca="false">SUM(AX3:AX38)/36</f>
+        <v>0.0277777777777778</v>
       </c>
       <c r="AY39" s="57" t="n">
-        <f aca="false">SUM(AY3:AY38)/23</f>
-        <v>0.0434782608695652</v>
+        <f aca="false">SUM(AY3:AY38)/36</f>
+        <v>0.0277777777777778</v>
       </c>
       <c r="AZ39" s="57" t="n">
-        <f aca="false">SUM(AZ3:AZ38)/23</f>
-        <v>0.217391304347826</v>
+        <f aca="false">SUM(AZ3:AZ38)/36</f>
+        <v>0.138888888888889</v>
       </c>
       <c r="BA39" s="57" t="n">
-        <f aca="false">SUM(BA3:BA38)/23</f>
-        <v>0.304347826086957</v>
+        <f aca="false">SUM(BA3:BA38)/36</f>
+        <v>0.194444444444444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>